<commit_message>
Removed NA# from Excel feedback so looks les like an error.
</commit_message>
<xml_diff>
--- a/www/PhotoElectricEffect.xlsx
+++ b/www/PhotoElectricEffect.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CaptProton/GitRepos/JAC_PHYS/PhotoelectricEffect/www/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E47A07-92D0-104E-B4DE-ABDF300F5C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4939B455-F18E-EB45-BFF3-2DDFFC6DB8CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{A8E1E6CA-66D9-5845-B54D-64F72881A8D5}"/>
   </bookViews>
@@ -329,7 +329,7 @@
     <numFmt numFmtId="165" formatCode="0E+00"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -372,6 +372,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -618,7 +624,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -626,142 +632,173 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -1134,22 +1171,30 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="E3" sqref="E3:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="6" width="11.83203125" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="8.83203125" customWidth="1"/>
+    <col min="10" max="11" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="23"/>
-      <c r="B1" s="40"/>
+      <c r="A1" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>15</v>
+      </c>
       <c r="C1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="43"/>
+      <c r="D1" s="20"/>
       <c r="E1" s="4" t="s">
         <v>20</v>
       </c>
@@ -1158,166 +1203,162 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
-      <c r="K1" s="24"/>
-    </row>
-    <row r="2" spans="1:11" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="47" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="K1" s="11"/>
+    </row>
+    <row r="2" spans="1:11" s="27" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="50"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="23" t="s">
         <v>18</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="F2" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="52" t="s">
+      <c r="G2" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="52" t="s">
+      <c r="H2" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="53" t="s">
+      <c r="I2" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="49" t="s">
+      <c r="J2" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="50" t="s">
+      <c r="K2" s="42" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="27"/>
-      <c r="B3" s="41" t="s">
+      <c r="A3" s="12"/>
+      <c r="B3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="26">
+      <c r="C3" s="1">
         <v>400</v>
       </c>
-      <c r="D3" s="44">
+      <c r="D3" s="21">
         <v>15</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="25" t="e">
-        <f>IF(COUNT(E3:I3)&gt;0,AVERAGE(E3:I3),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K3" s="30" t="e">
-        <f>IF(COUNT(E3:I3)&gt;2,_xlfn.STDEV.S(E3:I3)/SQRT(COUNT(E3:I3)),NA())</f>
-        <v>#N/A</v>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="27" t="str">
+        <f>IF(COUNT(E3:I3)&gt;0,AVERAGE(E3:I3),"—")</f>
+        <v>—</v>
+      </c>
+      <c r="K3" s="29" t="str">
+        <f>IF(COUNT(E3:I3)=1,0,IF(COUNT(E3:I3)&gt;2,_xlfn.STDEV.S(E3:I3)/SQRT(COUNT(E3:I3)),"—"))</f>
+        <v>—</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="31"/>
-      <c r="B4" s="41" t="s">
+      <c r="A4" s="13"/>
+      <c r="B4" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="26">
+      <c r="C4" s="1">
         <v>460</v>
       </c>
-      <c r="D4" s="44">
+      <c r="D4" s="21">
         <v>25</v>
       </c>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="25" t="e">
-        <f t="shared" ref="J4:J7" si="0">IF(COUNT(E4:I4)&gt;0,AVERAGE(E4:I4),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K4" s="30" t="e">
-        <f t="shared" ref="K4:K7" si="1">IF(COUNT(E4:I4)&gt;2,_xlfn.STDEV.S(E4:I4)/SQRT(COUNT(E4:I4)),NA())</f>
-        <v>#N/A</v>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="27" t="str">
+        <f t="shared" ref="J4:J7" si="0">IF(COUNT(E4:I4)&gt;0,AVERAGE(E4:I4),"—")</f>
+        <v>—</v>
+      </c>
+      <c r="K4" s="29" t="str">
+        <f t="shared" ref="K4:K7" si="1">IF(COUNT(E4:I4)=1,0,IF(COUNT(E4:I4)&gt;2,_xlfn.STDEV.S(E4:I4)/SQRT(COUNT(E4:I4)),"—"))</f>
+        <v>—</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="32"/>
-      <c r="B5" s="41" t="s">
+      <c r="A5" s="14"/>
+      <c r="B5" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="26">
+      <c r="C5" s="1">
         <v>520</v>
       </c>
-      <c r="D5" s="44">
+      <c r="D5" s="21">
         <v>35</v>
       </c>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="25" t="e">
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="K5" s="30" t="e">
+        <v>—</v>
+      </c>
+      <c r="K5" s="29" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>—</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="33"/>
-      <c r="B6" s="41" t="s">
+      <c r="A6" s="15"/>
+      <c r="B6" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="1">
         <v>610</v>
       </c>
-      <c r="D6" s="44">
+      <c r="D6" s="21">
         <v>17</v>
       </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="25" t="e">
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="K6" s="30" t="e">
+        <v>—</v>
+      </c>
+      <c r="K6" s="29" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>—</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" s="42" t="s">
+      <c r="A7" s="16"/>
+      <c r="B7" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="36">
+      <c r="C7" s="17">
         <v>660</v>
       </c>
-      <c r="D7" s="45">
+      <c r="D7" s="22">
         <v>25</v>
       </c>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="35" t="e">
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="K7" s="39" t="e">
+        <v>—</v>
+      </c>
+      <c r="K7" s="30" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>—</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1343,157 +1384,157 @@
       <c r="A10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="10" t="s">
         <v>17</v>
       </c>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="12">
+      <c r="A11" s="38">
         <f>IF(ISNUMBER(C3),299792458/C3*1000000000,"")</f>
         <v>749481145000000</v>
       </c>
-      <c r="B11" s="13" t="e">
-        <f>IF(ISNUMBER(E3),E3,NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C11" s="13" t="e">
-        <f>IF(ISNUMBER(E3),E3*1.602176634E-19,NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D11" s="14">
+      <c r="B11" s="31" t="str">
+        <f>IF(ISNUMBER(E3),E3,"—")</f>
+        <v>—</v>
+      </c>
+      <c r="C11" s="31" t="str">
+        <f>IF(ISNUMBER(E3),E3*1.602176634E-19,"—")</f>
+        <v>—</v>
+      </c>
+      <c r="D11" s="39">
         <f>D3/C3*A11</f>
         <v>28105542937500</v>
       </c>
-      <c r="E11" s="15" t="e">
-        <f>IF(ISNUMBER(K3),K3,NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F11" s="16" t="e">
-        <f>IF(ISNUMBER(E11),E11*1.602176634E-19,NA())</f>
-        <v>#N/A</v>
+      <c r="E11" s="33" t="str">
+        <f>IF(ISNUMBER(K3),K3,"—")</f>
+        <v>—</v>
+      </c>
+      <c r="F11" s="34" t="str">
+        <f>IF(ISNUMBER(E11),E11*1.602176634E-19,"—")</f>
+        <v>—</v>
       </c>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="12">
+      <c r="A12" s="38">
         <f t="shared" ref="A12:A15" si="2">IF(ISNUMBER(C4),299792458/C4*1000000000,"")</f>
         <v>651722734782608.75</v>
       </c>
-      <c r="B12" s="13" t="e">
-        <f t="shared" ref="B12:B15" si="3">IF(ISNUMBER(E4),E4,NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C12" s="13" t="e">
-        <f t="shared" ref="C12:C15" si="4">IF(ISNUMBER(E4),E4*1.602176634E-19,NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D12" s="14">
+      <c r="B12" s="31" t="str">
+        <f t="shared" ref="B12:B15" si="3">IF(ISNUMBER(E4),E4,"—")</f>
+        <v>—</v>
+      </c>
+      <c r="C12" s="31" t="str">
+        <f t="shared" ref="C12:C15" si="4">IF(ISNUMBER(E4),E4*1.602176634E-19,"—")</f>
+        <v>—</v>
+      </c>
+      <c r="D12" s="39">
         <f t="shared" ref="D12:D15" si="5">D4/C4*A12</f>
         <v>35419713846880.906</v>
       </c>
-      <c r="E12" s="13" t="e">
-        <f t="shared" ref="E12:E15" si="6">IF(ISNUMBER(K4),K4,NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F12" s="17" t="e">
-        <f t="shared" ref="F12:F15" si="7">IF(ISNUMBER(E12),E12*1.602176634E-19,NA())</f>
-        <v>#N/A</v>
+      <c r="E12" s="31" t="str">
+        <f t="shared" ref="E12:E15" si="6">IF(ISNUMBER(K4),K4,"—")</f>
+        <v>—</v>
+      </c>
+      <c r="F12" s="35" t="str">
+        <f t="shared" ref="F12:F15" si="7">IF(ISNUMBER(E12),E12*1.602176634E-19,"—")</f>
+        <v>—</v>
       </c>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="12">
+      <c r="A13" s="38">
         <f t="shared" si="2"/>
         <v>576523957692307.62</v>
       </c>
-      <c r="B13" s="13" t="e">
+      <c r="B13" s="31" t="str">
         <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-      <c r="C13" s="13" t="e">
+        <v>—</v>
+      </c>
+      <c r="C13" s="31" t="str">
         <f t="shared" si="4"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D13" s="14">
+        <v>—</v>
+      </c>
+      <c r="D13" s="39">
         <f t="shared" si="5"/>
         <v>38804497152366.859</v>
       </c>
-      <c r="E13" s="13" t="e">
+      <c r="E13" s="31" t="str">
         <f t="shared" si="6"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F13" s="17" t="e">
+        <v>—</v>
+      </c>
+      <c r="F13" s="35" t="str">
         <f t="shared" si="7"/>
-        <v>#N/A</v>
+        <v>—</v>
       </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="12">
+      <c r="A14" s="38">
         <f t="shared" si="2"/>
         <v>491463045901639.31</v>
       </c>
-      <c r="B14" s="13" t="e">
+      <c r="B14" s="31" t="str">
         <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-      <c r="C14" s="13" t="e">
+        <v>—</v>
+      </c>
+      <c r="C14" s="31" t="str">
         <f t="shared" si="4"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D14" s="14">
+        <v>—</v>
+      </c>
+      <c r="D14" s="39">
         <f t="shared" si="5"/>
         <v>13696511115291.588</v>
       </c>
-      <c r="E14" s="13" t="e">
+      <c r="E14" s="31" t="str">
         <f t="shared" si="6"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F14" s="18" t="e">
+        <v>—</v>
+      </c>
+      <c r="F14" s="36" t="str">
         <f t="shared" si="7"/>
-        <v>#N/A</v>
+        <v>—</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="19">
+      <c r="A15" s="40">
         <f t="shared" si="2"/>
         <v>454230996969696.94</v>
       </c>
-      <c r="B15" s="20" t="e">
+      <c r="B15" s="32" t="str">
         <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-      <c r="C15" s="20" t="e">
+        <v>—</v>
+      </c>
+      <c r="C15" s="32" t="str">
         <f t="shared" si="4"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D15" s="21">
+        <v>—</v>
+      </c>
+      <c r="D15" s="41">
         <f t="shared" si="5"/>
         <v>17205719582185.49</v>
       </c>
-      <c r="E15" s="20" t="e">
+      <c r="E15" s="32" t="str">
         <f t="shared" si="6"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F15" s="22" t="e">
+        <v>—</v>
+      </c>
+      <c r="F15" s="37" t="str">
         <f t="shared" si="7"/>
-        <v>#N/A</v>
+        <v>—</v>
       </c>
       <c r="G15" s="1"/>
     </row>
@@ -1525,14 +1566,18 @@
       <c r="G24" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="P6q1pW2CFnRhyD88uJwv65KiWLbgP6HbG89Y0N+0VxCow7c3joL2KC6jYkiyS2cP+wKxxwPNoOlOdqvEtSdtpA==" saltValue="IozVEEAbOR+mMh3v1u/zKA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+  </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="C3:D5">
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>T3&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:D7">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>V6&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1548,7 +1593,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="J3:K7" formulaRange="1"/>
+    <ignoredError sqref="J4:J7 J3 K3:K7" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Post Excel work clean-up
</commit_message>
<xml_diff>
--- a/www/PhotoElectricEffect.xlsx
+++ b/www/PhotoElectricEffect.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CaptProton/GitRepos/JAC_PHYS/PhotoelectricEffect/www/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4939B455-F18E-EB45-BFF3-2DDFFC6DB8CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007B26E5-9941-9E43-9641-A19471174FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{A8E1E6CA-66D9-5845-B54D-64F72881A8D5}"/>
   </bookViews>
@@ -1171,7 +1171,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:I7"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1566,6 +1566,7 @@
       <c r="G24" s="1"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="qsEM/UtHtR8Hg/eAv6jXr7V3ZK01/sR9rooLXG3lyS6AIxRu6bCSPzULHohUgQHSLV/Hk/LNXGfcqpTzlcjtiw==" saltValue="06iwkhyORUl2/NwaUq/oJQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>

</xml_diff>

<commit_message>
Further fixes to the Excel file.
</commit_message>
<xml_diff>
--- a/www/PhotoElectricEffect.xlsx
+++ b/www/PhotoElectricEffect.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CaptProton/GitRepos/JAC_PHYS/PhotoelectricEffect/www/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007B26E5-9941-9E43-9641-A19471174FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35545B8-92D3-B04D-B73B-BC2822E77A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{A8E1E6CA-66D9-5845-B54D-64F72881A8D5}"/>
   </bookViews>
@@ -778,27 +778,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -1171,14 +1151,14 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="E3" sqref="E3:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
     <col min="5" max="9" width="8.83203125" customWidth="1"/>
     <col min="10" max="11" width="10.83203125" customWidth="1"/>
@@ -1407,12 +1387,11 @@
         <v>749481145000000</v>
       </c>
       <c r="B11" s="31" t="str">
-        <f>IF(ISNUMBER(E3),E3,"—")</f>
-        <v>—</v>
-      </c>
-      <c r="C11" s="31" t="str">
-        <f>IF(ISNUMBER(E3),E3*1.602176634E-19,"—")</f>
-        <v>—</v>
+        <f>IF(ISNUMBER(J3),J3,"—")</f>
+        <v>—</v>
+      </c>
+      <c r="C11" s="31">
+        <v>2.9437752602462397E-19</v>
       </c>
       <c r="D11" s="39">
         <f>D3/C3*A11</f>
@@ -1434,23 +1413,22 @@
         <v>651722734782608.75</v>
       </c>
       <c r="B12" s="31" t="str">
-        <f t="shared" ref="B12:B15" si="3">IF(ISNUMBER(E4),E4,"—")</f>
-        <v>—</v>
-      </c>
-      <c r="C12" s="31" t="str">
-        <f t="shared" ref="C12:C15" si="4">IF(ISNUMBER(E4),E4*1.602176634E-19,"—")</f>
-        <v>—</v>
+        <f t="shared" ref="B12:B15" si="3">IF(ISNUMBER(J4),J4,"—")</f>
+        <v>—</v>
+      </c>
+      <c r="C12" s="31">
+        <v>2.9437752602462397E-19</v>
       </c>
       <c r="D12" s="39">
-        <f t="shared" ref="D12:D15" si="5">D4/C4*A12</f>
+        <f t="shared" ref="D12:D15" si="4">D4/C4*A12</f>
         <v>35419713846880.906</v>
       </c>
       <c r="E12" s="31" t="str">
-        <f t="shared" ref="E12:E15" si="6">IF(ISNUMBER(K4),K4,"—")</f>
+        <f t="shared" ref="E12:E15" si="5">IF(ISNUMBER(K4),K4,"—")</f>
         <v>—</v>
       </c>
       <c r="F12" s="35" t="str">
-        <f t="shared" ref="F12:F15" si="7">IF(ISNUMBER(E12),E12*1.602176634E-19,"—")</f>
+        <f t="shared" ref="F12:F15" si="6">IF(ISNUMBER(E12),E12*1.602176634E-19,"—")</f>
         <v>—</v>
       </c>
       <c r="G12" s="1"/>
@@ -1464,20 +1442,19 @@
         <f t="shared" si="3"/>
         <v>—</v>
       </c>
-      <c r="C13" s="31" t="str">
+      <c r="C13" s="31">
+        <v>2.9437752602462397E-19</v>
+      </c>
+      <c r="D13" s="39">
         <f t="shared" si="4"/>
-        <v>—</v>
-      </c>
-      <c r="D13" s="39">
+        <v>38804497152366.859</v>
+      </c>
+      <c r="E13" s="31" t="str">
         <f t="shared" si="5"/>
-        <v>38804497152366.859</v>
-      </c>
-      <c r="E13" s="31" t="str">
+        <v>—</v>
+      </c>
+      <c r="F13" s="35" t="str">
         <f t="shared" si="6"/>
-        <v>—</v>
-      </c>
-      <c r="F13" s="35" t="str">
-        <f t="shared" si="7"/>
         <v>—</v>
       </c>
       <c r="G13" s="1"/>
@@ -1491,20 +1468,19 @@
         <f t="shared" si="3"/>
         <v>—</v>
       </c>
-      <c r="C14" s="31" t="str">
+      <c r="C14" s="31">
+        <v>2.9437752602462397E-19</v>
+      </c>
+      <c r="D14" s="39">
         <f t="shared" si="4"/>
-        <v>—</v>
-      </c>
-      <c r="D14" s="39">
+        <v>13696511115291.588</v>
+      </c>
+      <c r="E14" s="31" t="str">
         <f t="shared" si="5"/>
-        <v>13696511115291.588</v>
-      </c>
-      <c r="E14" s="31" t="str">
+        <v>—</v>
+      </c>
+      <c r="F14" s="36" t="str">
         <f t="shared" si="6"/>
-        <v>—</v>
-      </c>
-      <c r="F14" s="36" t="str">
-        <f t="shared" si="7"/>
         <v>—</v>
       </c>
       <c r="G14" s="1"/>
@@ -1520,20 +1496,19 @@
         <f t="shared" si="3"/>
         <v>—</v>
       </c>
-      <c r="C15" s="32" t="str">
+      <c r="C15" s="32">
+        <v>2.9437752602462397E-19</v>
+      </c>
+      <c r="D15" s="41">
         <f t="shared" si="4"/>
-        <v>—</v>
-      </c>
-      <c r="D15" s="41">
+        <v>17205719582185.49</v>
+      </c>
+      <c r="E15" s="32" t="str">
         <f t="shared" si="5"/>
-        <v>17205719582185.49</v>
-      </c>
-      <c r="E15" s="32" t="str">
+        <v>—</v>
+      </c>
+      <c r="F15" s="37" t="str">
         <f t="shared" si="6"/>
-        <v>—</v>
-      </c>
-      <c r="F15" s="37" t="str">
-        <f t="shared" si="7"/>
         <v>—</v>
       </c>
       <c r="G15" s="1"/>
@@ -1566,19 +1541,19 @@
       <c r="G24" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="qsEM/UtHtR8Hg/eAv6jXr7V3ZK01/sR9rooLXG3lyS6AIxRu6bCSPzULHohUgQHSLV/Hk/LNXGfcqpTzlcjtiw==" saltValue="06iwkhyORUl2/NwaUq/oJQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="CJQKfqvWKDXl1tVpxOaTL9hNWOEXe2ao3o0Zr8SsQ4ARLf77aqoEOuG47j3znK22rBFbfGHhR6tw+DXPqn8ZLA==" saltValue="Ozw5vy/kyG/ChduJ68p5Qg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="C3:D5">
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="2" priority="6">
       <formula>T3&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:D7">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>V6&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>